<commit_message>
doc: Convert html table to markdown table in README.md
</commit_message>
<xml_diff>
--- a/misc/Component properties.xlsx
+++ b/misc/Component properties.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogasimli\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogasimli\Documents\GitHub\My Projects\HealthBarView\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
   <si>
     <t>integer</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Property</t>
+  </si>
+  <si>
+    <t>Component</t>
   </si>
 </sst>
 </file>
@@ -207,13 +210,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,320 +536,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="b">
+      <c r="D7" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="b">
+      <c r="D22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="C23" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="D23" s="1">
         <v>4000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A27:C27"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>